<commit_message>
use CSTR instead of PFR
</commit_message>
<xml_diff>
--- a/exposan/bsm2/data/bsm2p_init.xlsx
+++ b/exposan/bsm2/data/bsm2p_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\bsm2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2264E944-8D18-4B17-B564-BEE3BEF5C6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CBC00F-5E5A-4ED7-B8B1-B5492476A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="24750" windowHeight="18450" activeTab="1" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="5160" yWindow="5640" windowWidth="21255" windowHeight="14700" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="asm" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
   <si>
     <t>S_O2</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>inf</t>
+  </si>
+  <si>
+    <t>X_CaCO3</t>
+  </si>
+  <si>
+    <t>X_newb</t>
+  </si>
+  <si>
+    <t>X_MgCO3</t>
+  </si>
+  <si>
+    <t>X_AlOH</t>
+  </si>
+  <si>
+    <t>X_AlPO4</t>
+  </si>
+  <si>
+    <t>X_FeOH</t>
   </si>
 </sst>
 </file>
@@ -275,10 +293,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,15 +632,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67887DCA-7CBD-4529-953E-A8DE039190F5}">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -685,8 +709,35 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -753,8 +804,35 @@
       <c r="V2" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -821,8 +899,35 @@
       <c r="V3" s="2">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -889,8 +994,35 @@
       <c r="V4">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -957,8 +1089,35 @@
       <c r="V5">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1025,8 +1184,35 @@
       <c r="V6">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1093,8 +1279,35 @@
       <c r="V7">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1161,8 +1374,35 @@
       <c r="V8">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1229,8 +1469,35 @@
       <c r="V9">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1297,58 +1564,35 @@
       <c r="V10">
         <v>118.9924</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="W10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="21:26" x14ac:dyDescent="0.25">
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
@@ -1366,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add test for mASM2d-ADM1p interface
</commit_message>
<xml_diff>
--- a/exposan/bsm2/data/bsm2p_init.xlsx
+++ b/exposan/bsm2/data/bsm2p_init.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\bsm2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CBC00F-5E5A-4ED7-B8B1-B5492476A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E723514F-97B2-487C-A96F-3E59C1F607D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="5640" windowWidth="21255" windowHeight="14700" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="29445" windowHeight="15345" activeTab="1" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="asm" sheetId="1" r:id="rId1"/>
-    <sheet name="adm" sheetId="2" r:id="rId2"/>
-    <sheet name="settler" sheetId="3" r:id="rId3"/>
-    <sheet name="others" sheetId="4" r:id="rId4"/>
+    <sheet name="asm2" sheetId="6" r:id="rId2"/>
+    <sheet name="adm" sheetId="2" r:id="rId3"/>
+    <sheet name="adm2" sheetId="5" r:id="rId4"/>
+    <sheet name="settler" sheetId="3" r:id="rId5"/>
+    <sheet name="others" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="71">
   <si>
     <t>S_O2</t>
   </si>
@@ -246,6 +248,12 @@
   </si>
   <si>
     <t>X_FeOH</t>
+  </si>
+  <si>
+    <t>S_h2</t>
+  </si>
+  <si>
+    <t>H2O</t>
   </si>
 </sst>
 </file>
@@ -634,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67887DCA-7CBD-4529-953E-A8DE039190F5}">
   <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,11 +1615,986 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84C1DB9-63E8-4585-98A4-57278B8222C3}">
+  <dimension ref="A1:AE20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2">
+        <v>57.45</v>
+      </c>
+      <c r="E2" s="2">
+        <v>26.6</v>
+      </c>
+      <c r="F2" s="2">
+        <v>25.19</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5.6520000000000001</v>
+      </c>
+      <c r="J2" s="2">
+        <v>84</v>
+      </c>
+      <c r="K2" s="2">
+        <v>94.1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>370</v>
+      </c>
+      <c r="M2" s="2">
+        <v>51.53</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>20</v>
+      </c>
+      <c r="S2" s="2">
+        <v>30</v>
+      </c>
+      <c r="T2" s="2">
+        <v>175</v>
+      </c>
+      <c r="U2" s="2">
+        <v>300</v>
+      </c>
+      <c r="V2" s="2">
+        <v>60</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>69.5852</v>
+      </c>
+      <c r="D3" s="2">
+        <v>57.004199999999997</v>
+      </c>
+      <c r="E3" s="2">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>34.576000000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.1991</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>14.0077</v>
+      </c>
+      <c r="J3" s="2">
+        <v>89.923000000000002</v>
+      </c>
+      <c r="K3" s="2">
+        <v>50.216799999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>224.4676</v>
+      </c>
+      <c r="M3" s="2">
+        <v>31.997499999999999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.47560000000000002</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.1394</v>
+      </c>
+      <c r="P3" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="R3" s="2">
+        <v>24.408999999999999</v>
+      </c>
+      <c r="S3" s="2">
+        <v>99.133399999999995</v>
+      </c>
+      <c r="T3" s="2">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U3" s="2">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V3" s="2">
+        <v>118.9924</v>
+      </c>
+      <c r="W3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>1E-3</v>
+      </c>
+      <c r="C4">
+        <v>4.9268999999999998</v>
+      </c>
+      <c r="D4">
+        <v>15.1297</v>
+      </c>
+      <c r="E4">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F4">
+        <v>18.388400000000001</v>
+      </c>
+      <c r="G4">
+        <v>8.7476000000000003</v>
+      </c>
+      <c r="H4">
+        <v>5.4899999999999997E-2</v>
+      </c>
+      <c r="I4">
+        <v>24.657699999999998</v>
+      </c>
+      <c r="J4">
+        <v>78.586799999999997</v>
+      </c>
+      <c r="K4">
+        <v>1823.9622999999999</v>
+      </c>
+      <c r="L4">
+        <v>131.804</v>
+      </c>
+      <c r="M4">
+        <v>1013</v>
+      </c>
+      <c r="N4">
+        <v>400</v>
+      </c>
+      <c r="O4">
+        <v>278.53640000000001</v>
+      </c>
+      <c r="P4">
+        <v>44.267299999999999</v>
+      </c>
+      <c r="Q4">
+        <v>55</v>
+      </c>
+      <c r="R4">
+        <v>28.996300000000002</v>
+      </c>
+      <c r="S4">
+        <v>101.9855</v>
+      </c>
+      <c r="T4">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U4">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V4">
+        <v>118.9924</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1.1234</v>
+      </c>
+      <c r="D5">
+        <v>4.6102999999999996</v>
+      </c>
+      <c r="E5">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F5">
+        <v>19.059200000000001</v>
+      </c>
+      <c r="G5">
+        <v>8.8010000000000002</v>
+      </c>
+      <c r="H5">
+        <v>1.5E-3</v>
+      </c>
+      <c r="I5">
+        <v>37.046599999999998</v>
+      </c>
+      <c r="J5">
+        <v>79.785799999999995</v>
+      </c>
+      <c r="K5">
+        <v>1823.9645</v>
+      </c>
+      <c r="L5">
+        <v>115.021</v>
+      </c>
+      <c r="M5">
+        <v>1014</v>
+      </c>
+      <c r="N5">
+        <v>400</v>
+      </c>
+      <c r="O5">
+        <v>266.25779999999997</v>
+      </c>
+      <c r="P5">
+        <v>74.996499999999997</v>
+      </c>
+      <c r="Q5">
+        <v>55</v>
+      </c>
+      <c r="R5">
+        <v>34.1586</v>
+      </c>
+      <c r="S5">
+        <v>105.1951</v>
+      </c>
+      <c r="T5">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U5">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V5">
+        <v>118.9924</v>
+      </c>
+      <c r="W5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.4798</v>
+      </c>
+      <c r="D6">
+        <v>0.22409999999999999</v>
+      </c>
+      <c r="E6">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F6">
+        <v>7.4791999999999996</v>
+      </c>
+      <c r="G6">
+        <v>13.0839</v>
+      </c>
+      <c r="H6">
+        <v>1.0373000000000001</v>
+      </c>
+      <c r="I6">
+        <v>12.245699999999999</v>
+      </c>
+      <c r="J6">
+        <v>69.465100000000007</v>
+      </c>
+      <c r="K6">
+        <v>1832.5407</v>
+      </c>
+      <c r="L6">
+        <v>62.077399999999997</v>
+      </c>
+      <c r="M6">
+        <v>1030</v>
+      </c>
+      <c r="N6">
+        <v>410</v>
+      </c>
+      <c r="O6">
+        <v>290.70609999999999</v>
+      </c>
+      <c r="P6">
+        <v>25.902899999999999</v>
+      </c>
+      <c r="Q6">
+        <v>56</v>
+      </c>
+      <c r="R6">
+        <v>23.879799999999999</v>
+      </c>
+      <c r="S6">
+        <v>98.804400000000001</v>
+      </c>
+      <c r="T6">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U6">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V6">
+        <v>118.9924</v>
+      </c>
+      <c r="W6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>1E-4</v>
+      </c>
+      <c r="C7">
+        <v>0.49080000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.3836</v>
+      </c>
+      <c r="E7">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F7">
+        <v>7.4557000000000002</v>
+      </c>
+      <c r="G7">
+        <v>13.952299999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="I7">
+        <v>12.051500000000001</v>
+      </c>
+      <c r="J7">
+        <v>70.103300000000004</v>
+      </c>
+      <c r="K7">
+        <v>1832.6564000000001</v>
+      </c>
+      <c r="L7">
+        <v>56.1325</v>
+      </c>
+      <c r="M7">
+        <v>1031</v>
+      </c>
+      <c r="N7">
+        <v>410</v>
+      </c>
+      <c r="O7">
+        <v>290.87889999999999</v>
+      </c>
+      <c r="P7">
+        <v>26.580500000000001</v>
+      </c>
+      <c r="Q7">
+        <v>56</v>
+      </c>
+      <c r="R7">
+        <v>23.807200000000002</v>
+      </c>
+      <c r="S7">
+        <v>98.759200000000007</v>
+      </c>
+      <c r="T7">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U7">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V7">
+        <v>118.9924</v>
+      </c>
+      <c r="W7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0.4078</v>
+      </c>
+      <c r="C8">
+        <v>0.34110000000000001</v>
+      </c>
+      <c r="D8">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F8">
+        <v>3.8313000000000001</v>
+      </c>
+      <c r="G8">
+        <v>12.9102</v>
+      </c>
+      <c r="H8">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="I8">
+        <v>3.1339999999999999</v>
+      </c>
+      <c r="J8">
+        <v>65.202399999999997</v>
+      </c>
+      <c r="K8">
+        <v>1834.2221</v>
+      </c>
+      <c r="L8">
+        <v>47.112699999999997</v>
+      </c>
+      <c r="M8">
+        <v>1033</v>
+      </c>
+      <c r="N8">
+        <v>413</v>
+      </c>
+      <c r="O8">
+        <v>299.64010000000002</v>
+      </c>
+      <c r="P8">
+        <v>9.6491000000000007</v>
+      </c>
+      <c r="Q8">
+        <v>56</v>
+      </c>
+      <c r="R8">
+        <v>20.123699999999999</v>
+      </c>
+      <c r="S8">
+        <v>96.469099999999997</v>
+      </c>
+      <c r="T8">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U8">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V8">
+        <v>118.9924</v>
+      </c>
+      <c r="W8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>1.1736</v>
+      </c>
+      <c r="C9">
+        <v>0.29909999999999998</v>
+      </c>
+      <c r="D9">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="E9">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.95520000000000005</v>
+      </c>
+      <c r="G9">
+        <v>12.477600000000001</v>
+      </c>
+      <c r="H9">
+        <v>4.4699</v>
+      </c>
+      <c r="I9">
+        <v>0.69189999999999996</v>
+      </c>
+      <c r="J9">
+        <v>60.955800000000004</v>
+      </c>
+      <c r="K9">
+        <v>1836.0331000000001</v>
+      </c>
+      <c r="L9">
+        <v>40.818800000000003</v>
+      </c>
+      <c r="M9">
+        <v>1033</v>
+      </c>
+      <c r="N9">
+        <v>413</v>
+      </c>
+      <c r="O9">
+        <v>302.08850000000001</v>
+      </c>
+      <c r="P9">
+        <v>2.4420999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>57</v>
+      </c>
+      <c r="R9">
+        <v>19.0943</v>
+      </c>
+      <c r="S9">
+        <v>95.829099999999997</v>
+      </c>
+      <c r="T9">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U9">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V9">
+        <v>118.9924</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>1.0591999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.311</v>
+      </c>
+      <c r="D10">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="E10">
+        <v>26.596299999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.23330000000000001</v>
+      </c>
+      <c r="G10">
+        <v>12.450100000000001</v>
+      </c>
+      <c r="H10">
+        <v>5.2125000000000004</v>
+      </c>
+      <c r="I10">
+        <v>0.8256</v>
+      </c>
+      <c r="J10">
+        <v>59.654000000000003</v>
+      </c>
+      <c r="K10">
+        <v>1837.8286000000001</v>
+      </c>
+      <c r="L10">
+        <v>36.499499999999998</v>
+      </c>
+      <c r="M10">
+        <v>1033</v>
+      </c>
+      <c r="N10">
+        <v>412</v>
+      </c>
+      <c r="O10">
+        <v>302.05119999999999</v>
+      </c>
+      <c r="P10">
+        <v>0.62460000000000004</v>
+      </c>
+      <c r="Q10">
+        <v>57</v>
+      </c>
+      <c r="R10">
+        <v>19.11</v>
+      </c>
+      <c r="S10">
+        <v>95.838800000000006</v>
+      </c>
+      <c r="T10">
+        <v>82.441500000000005</v>
+      </c>
+      <c r="U10">
+        <v>449.95940000000002</v>
+      </c>
+      <c r="V10">
+        <v>118.9924</v>
+      </c>
+      <c r="W10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="X10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="21:26" x14ac:dyDescent="0.25">
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,7 +2812,285 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADEEAAA-987D-43CA-A836-37D3B86B2368}">
+  <dimension ref="A1:AQ2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C2">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="D2">
+        <v>0.126</v>
+      </c>
+      <c r="E2">
+        <v>1.29E-2</v>
+      </c>
+      <c r="F2">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="G2">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="H2">
+        <v>5.8799999999999998E-2</v>
+      </c>
+      <c r="I2">
+        <v>2.8308999999999998E-7</v>
+      </c>
+      <c r="J2">
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="K2">
+        <f>0.089*12</f>
+        <v>1.0680000000000001</v>
+      </c>
+      <c r="L2">
+        <f>0.0663*14</f>
+        <v>0.92819999999999991</v>
+      </c>
+      <c r="M2">
+        <f>0.028*31</f>
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="N2">
+        <v>2.63E-2</v>
+      </c>
+      <c r="O2">
+        <v>1.302</v>
+      </c>
+      <c r="P2">
+        <v>1.3613</v>
+      </c>
+      <c r="Q2">
+        <v>1.8127</v>
+      </c>
+      <c r="R2">
+        <v>0.51459999999999995</v>
+      </c>
+      <c r="S2">
+        <v>0.4017</v>
+      </c>
+      <c r="T2">
+        <v>0.37490000000000001</v>
+      </c>
+      <c r="U2">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="V2">
+        <v>8.9599999999999999E-2</v>
+      </c>
+      <c r="W2">
+        <v>0.50060000000000004</v>
+      </c>
+      <c r="X2">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="Y2">
+        <v>12.9232</v>
+      </c>
+      <c r="Z2">
+        <v>0.66969999999999996</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="AC2">
+        <v>1.29E-2</v>
+      </c>
+      <c r="AD2">
+        <v>1E-4</v>
+      </c>
+      <c r="AE2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <f>0.0161</f>
+        <v>1.61E-2</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>1E-3</v>
+      </c>
+      <c r="AO2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AP2">
+        <v>1.26E-2</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA96946B-17C1-41F5-A32B-CE0A064A22AA}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -2017,7 +3278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AABAC6-0393-4FAA-A818-3D4621797738}">
   <dimension ref="B1:H13"/>
   <sheetViews>

</xml_diff>